<commit_message>
Added information about github classroom and link to the first assignment
</commit_message>
<xml_diff>
--- a/data-and-files/schedule_part2.xlsx
+++ b/data-and-files/schedule_part2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/repositories/ban400/data-and-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s12203\repos\ban400\data-and-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D2DBD8-68F2-764D-A3B9-E26F87AA2D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E433B8-25E5-4156-98B5-EF1A06A2B185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="17520" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -107,9 +107,6 @@
     <t>PWC</t>
   </si>
   <si>
-    <t>Git</t>
-  </si>
-  <si>
     <t>Iterations</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t>[Git](https://classroom.github.com/a/ojZuXTA9)</t>
   </si>
 </sst>
 </file>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,23 +523,23 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="5" max="5" width="32.125" customWidth="1"/>
     <col min="6" max="6" width="30.5" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>39</v>
       </c>
@@ -574,16 +574,16 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>40</v>
       </c>
@@ -597,10 +597,10 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>41</v>
       </c>
@@ -614,16 +614,16 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>42</v>
       </c>
@@ -637,16 +637,16 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>43</v>
       </c>
@@ -660,16 +660,16 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>44</v>
       </c>
@@ -683,16 +683,16 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>45</v>
       </c>
@@ -706,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added link for the final assignments
</commit_message>
<xml_diff>
--- a/data-and-files/schedule_part2.xlsx
+++ b/data-and-files/schedule_part2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nhh\ban400\data-and-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s12203\repos\ban400\data-and-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4420D69E-83DE-45FF-83EC-360DAD5B9F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32AAA8B-FE08-4BFE-910C-38D051482AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
+    <workbookView xWindow="35355" yWindow="135" windowWidth="19110" windowHeight="17145" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -107,12 +107,6 @@
     <t>PWC</t>
   </si>
   <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>Many models</t>
-  </si>
-  <si>
     <t>28.09 *08:15 - 10:00* (**Aud J**)</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>[Iterations](https://classroom.github.com/a/mJpP5ERB)</t>
+  </si>
+  <si>
+    <t>[Machine Learning](https://classroom.github.com/a/WRI89Flt)</t>
+  </si>
+  <si>
+    <t>[Many models](https://classroom.github.com/a/04gGD6TJ)</t>
   </si>
 </sst>
 </file>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,10 +523,10 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -539,7 +539,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -574,13 +574,13 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -614,13 +614,13 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -637,13 +637,13 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -660,13 +660,13 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -683,13 +683,13 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added links to most github assignments
</commit_message>
<xml_diff>
--- a/data-and-files/schedule_part2.xlsx
+++ b/data-and-files/schedule_part2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakon/work/repos/ban400/data-and-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575A169-3B5F-A14A-871F-56CB47221B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA57C6E-9210-284D-84CC-04F058BF9277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43760" yWindow="-940" windowWidth="19420" windowHeight="10420" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
+    <workbookView xWindow="43760" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{E8DA2206-E191-394A-AC89-C46277787FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -101,21 +101,6 @@
     <t>[Many models](10-many-models.qmd) and [Making maps](12-making-maps.qmd)</t>
   </si>
   <si>
-    <t>Git</t>
-  </si>
-  <si>
-    <t>Iterations</t>
-  </si>
-  <si>
-    <t>Parallel computing</t>
-  </si>
-  <si>
-    <t>Machine learning</t>
-  </si>
-  <si>
-    <t>Many Models/Making maps</t>
-  </si>
-  <si>
     <t>08.10.2024  (*07:00*)</t>
   </si>
   <si>
@@ -147,6 +132,21 @@
   </si>
   <si>
     <t>07:11 *08:15 - 10:00* (**LAB2**)</t>
+  </si>
+  <si>
+    <t>[Git](https://classroom.github.com/a/MkPXmUFj)</t>
+  </si>
+  <si>
+    <t>[Machine learning](https://classroom.github.com/a/W8Y8nIDh)</t>
+  </si>
+  <si>
+    <t>[Iterations](https://classroom.github.com/a/axYOETtq)</t>
+  </si>
+  <si>
+    <t>[Parallel computing](https://classroom.github.com/a/_w48Vu_p)</t>
+  </si>
+  <si>
+    <t>[Many Models](https://classroom.github.com/a/oNJOK_ws)/Making maps</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,13 +562,13 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -585,13 +585,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -608,13 +608,13 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -631,13 +631,13 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -654,13 +654,13 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>